<commit_message>
compare excel file updated
</commit_message>
<xml_diff>
--- a/compare-mnist.xlsx
+++ b/compare-mnist.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="109">
   <si>
     <t>step=</t>
   </si>
@@ -329,6 +330,28 @@
   </si>
   <si>
     <t>SDProp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>loss=</t>
+  </si>
+  <si>
+    <t>acc=</t>
+  </si>
+  <si>
+    <t>Adam Loss</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Adam Acc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDProp Loss</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDProp Acc</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -336,7 +359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -347,6 +370,24 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -370,14 +411,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -650,11 +711,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2147006664"/>
-        <c:axId val="-2132791256"/>
+        <c:axId val="2140572184"/>
+        <c:axId val="2140609176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2147006664"/>
+        <c:axId val="2140572184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +724,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132791256"/>
+        <c:crossAx val="2140609176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -671,8 +732,330 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132791256"/>
+        <c:axId val="2140609176"/>
         <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140572184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adam Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>565.45734</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.185616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.78059</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.144241</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.758614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.25866</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.17146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.063127</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.2274475</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.637199000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.376772</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.041093</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.754768</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.110620000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.3511033</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2841954</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.884306</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.515066</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.437247</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.600502</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.127358</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.3089924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5774632</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.162725</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.4844575</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.1178436</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.926961</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.442167</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6591474</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.515431</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SDProp Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$K$2:$K$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>472.33603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.73349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.761047</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.407032</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.546188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.092958</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.823841</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.437433</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.4117303</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.445073</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.841881</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.820187</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.839632</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.6102543</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.938401000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.6252804</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.3085408</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1648536</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.679963000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.2759576</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.4800506</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.191964</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9176717</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.5200233</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.6826854</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.359622</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.6358855</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8152013</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3718376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2146118024"/>
+        <c:axId val="2146121112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2146118024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146121112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2146121112"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -682,7 +1065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2147006664"/>
+        <c:crossAx val="2146118024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -708,16 +1091,51 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1064,7 +1482,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F32" sqref="F32:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1910,6 +2328,1254 @@
         <v>66</v>
       </c>
       <c r="G36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M36"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K1" activeCellId="1" sqref="D1:D31 K1:K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2">
+        <v>565.45734000000004</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2">
+        <v>472.33602999999999</v>
+      </c>
+      <c r="L2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2">
+        <v>0.1328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3">
+        <v>68.185615999999996</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3">
+        <v>0.84709999999999996</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3">
+        <v>87.733490000000003</v>
+      </c>
+      <c r="L3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3">
+        <v>0.7208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4">
+        <v>39.780589999999997</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4">
+        <v>0.9103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>200</v>
+      </c>
+      <c r="J4" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4">
+        <v>54.761046999999998</v>
+      </c>
+      <c r="L4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4">
+        <v>0.83930000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5">
+        <v>30.144241000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5">
+        <v>0.92879999999999996</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>300</v>
+      </c>
+      <c r="J5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5">
+        <v>45.482999999999997</v>
+      </c>
+      <c r="L5" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5">
+        <v>0.88160000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6">
+        <v>27.758614000000001</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6">
+        <v>0.93840000000000001</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>400</v>
+      </c>
+      <c r="J6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6">
+        <v>28.407032000000001</v>
+      </c>
+      <c r="L6" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6">
+        <v>0.91559999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7">
+        <v>12.258660000000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7">
+        <v>0.94710000000000005</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+      <c r="J7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7">
+        <v>18.546188000000001</v>
+      </c>
+      <c r="L7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7">
+        <v>0.92210000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>600</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8">
+        <v>12.17146</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8">
+        <v>0.95020000000000004</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>600</v>
+      </c>
+      <c r="J8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8">
+        <v>20.092957999999999</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>700</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9">
+        <v>13.063127</v>
+      </c>
+      <c r="E9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9">
+        <v>0.95589999999999997</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>700</v>
+      </c>
+      <c r="J9" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9">
+        <v>17.823841000000002</v>
+      </c>
+      <c r="L9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9">
+        <v>0.94169999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>800</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10">
+        <v>13.2274475</v>
+      </c>
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>800</v>
+      </c>
+      <c r="J10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10">
+        <v>20.437432999999999</v>
+      </c>
+      <c r="L10" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10">
+        <v>0.94850000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>900</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11">
+        <v>9.6371990000000007</v>
+      </c>
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11">
+        <v>0.96279999999999999</v>
+      </c>
+      <c r="H11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>900</v>
+      </c>
+      <c r="J11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11">
+        <v>7.4117303000000003</v>
+      </c>
+      <c r="L11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11">
+        <v>0.95640000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12">
+        <v>6.3767719999999999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12">
+        <v>0.96689999999999998</v>
+      </c>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1000</v>
+      </c>
+      <c r="J12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12">
+        <v>14.445073000000001</v>
+      </c>
+      <c r="L12" t="s">
+        <v>104</v>
+      </c>
+      <c r="M12">
+        <v>0.96209999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13">
+        <v>13.041093</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13">
+        <v>0.96750000000000003</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1100</v>
+      </c>
+      <c r="J13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13">
+        <v>10.841881000000001</v>
+      </c>
+      <c r="L13" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13">
+        <v>0.96399999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1200</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14">
+        <v>20.754767999999999</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14">
+        <v>0.97009999999999996</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1200</v>
+      </c>
+      <c r="J14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14">
+        <v>16.820187000000001</v>
+      </c>
+      <c r="L14" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14">
+        <v>0.96830000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1300</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15">
+        <v>9.1106200000000008</v>
+      </c>
+      <c r="E15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15">
+        <v>0.96930000000000005</v>
+      </c>
+      <c r="H15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1300</v>
+      </c>
+      <c r="J15" t="s">
+        <v>103</v>
+      </c>
+      <c r="K15">
+        <v>8.8396319999999999</v>
+      </c>
+      <c r="L15" t="s">
+        <v>104</v>
+      </c>
+      <c r="M15">
+        <v>0.97040000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1400</v>
+      </c>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16">
+        <v>7.3511033000000001</v>
+      </c>
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1400</v>
+      </c>
+      <c r="J16" t="s">
+        <v>103</v>
+      </c>
+      <c r="K16">
+        <v>7.6102543000000002</v>
+      </c>
+      <c r="L16" t="s">
+        <v>104</v>
+      </c>
+      <c r="M16">
+        <v>0.96679999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1500</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17">
+        <v>2.2841954000000002</v>
+      </c>
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17">
+        <v>0.97040000000000004</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1500</v>
+      </c>
+      <c r="J17" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17">
+        <v>9.9384010000000007</v>
+      </c>
+      <c r="L17" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17">
+        <v>0.97360000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1600</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18">
+        <v>10.884306</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18">
+        <v>0.97389999999999999</v>
+      </c>
+      <c r="H18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1600</v>
+      </c>
+      <c r="J18" t="s">
+        <v>103</v>
+      </c>
+      <c r="K18">
+        <v>5.6252804000000003</v>
+      </c>
+      <c r="L18" t="s">
+        <v>104</v>
+      </c>
+      <c r="M18">
+        <v>0.9748</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1700</v>
+      </c>
+      <c r="C19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19">
+        <v>17.515066000000001</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19">
+        <v>0.97509999999999997</v>
+      </c>
+      <c r="H19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1700</v>
+      </c>
+      <c r="J19" t="s">
+        <v>103</v>
+      </c>
+      <c r="K19">
+        <v>2.3085407999999998</v>
+      </c>
+      <c r="L19" t="s">
+        <v>104</v>
+      </c>
+      <c r="M19">
+        <v>0.97650000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1800</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20">
+        <v>9.4372469999999993</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20">
+        <v>0.97550000000000003</v>
+      </c>
+      <c r="H20" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1800</v>
+      </c>
+      <c r="J20" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20">
+        <v>1.1648536</v>
+      </c>
+      <c r="L20" t="s">
+        <v>104</v>
+      </c>
+      <c r="M20">
+        <v>0.97629999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1900</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21">
+        <v>8.6005020000000005</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21">
+        <v>0.97509999999999997</v>
+      </c>
+      <c r="H21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1900</v>
+      </c>
+      <c r="J21" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21">
+        <v>8.6799630000000008</v>
+      </c>
+      <c r="L21" t="s">
+        <v>104</v>
+      </c>
+      <c r="M21">
+        <v>0.97870000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>2000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22">
+        <v>3.1273580000000001</v>
+      </c>
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22">
+        <v>0.97789999999999999</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>2000</v>
+      </c>
+      <c r="J22" t="s">
+        <v>103</v>
+      </c>
+      <c r="K22">
+        <v>7.2759575999999999</v>
+      </c>
+      <c r="L22" t="s">
+        <v>104</v>
+      </c>
+      <c r="M22">
+        <v>0.97850000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>2100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23">
+        <v>4.3089924000000002</v>
+      </c>
+      <c r="E23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="H23" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>2100</v>
+      </c>
+      <c r="J23" t="s">
+        <v>103</v>
+      </c>
+      <c r="K23">
+        <v>5.4800506000000002</v>
+      </c>
+      <c r="L23" t="s">
+        <v>104</v>
+      </c>
+      <c r="M23">
+        <v>0.97929999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>2200</v>
+      </c>
+      <c r="C24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24">
+        <v>2.5774632</v>
+      </c>
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24">
+        <v>0.97760000000000002</v>
+      </c>
+      <c r="H24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>2200</v>
+      </c>
+      <c r="J24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K24">
+        <v>6.1919639999999996</v>
+      </c>
+      <c r="L24" t="s">
+        <v>104</v>
+      </c>
+      <c r="M24">
+        <v>0.97960000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>2300</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25">
+        <v>12.162725</v>
+      </c>
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25">
+        <v>0.9788</v>
+      </c>
+      <c r="H25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>2300</v>
+      </c>
+      <c r="J25" t="s">
+        <v>103</v>
+      </c>
+      <c r="K25">
+        <v>0.91767169999999998</v>
+      </c>
+      <c r="L25" t="s">
+        <v>104</v>
+      </c>
+      <c r="M25">
+        <v>0.98170000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>2400</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26">
+        <v>3.4844575</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26">
+        <v>0.97919999999999996</v>
+      </c>
+      <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>2400</v>
+      </c>
+      <c r="J26" t="s">
+        <v>103</v>
+      </c>
+      <c r="K26">
+        <v>6.5200233000000001</v>
+      </c>
+      <c r="L26" t="s">
+        <v>104</v>
+      </c>
+      <c r="M26">
+        <v>0.98129999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>2500</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27">
+        <v>6.1178435999999996</v>
+      </c>
+      <c r="E27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="H27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>2500</v>
+      </c>
+      <c r="J27" t="s">
+        <v>103</v>
+      </c>
+      <c r="K27">
+        <v>2.6826854</v>
+      </c>
+      <c r="L27" t="s">
+        <v>104</v>
+      </c>
+      <c r="M27">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>2600</v>
+      </c>
+      <c r="C28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28">
+        <v>6.9269610000000004</v>
+      </c>
+      <c r="E28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28">
+        <v>0.98060000000000003</v>
+      </c>
+      <c r="H28" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>2600</v>
+      </c>
+      <c r="J28" t="s">
+        <v>103</v>
+      </c>
+      <c r="K28">
+        <v>5.3596219999999999</v>
+      </c>
+      <c r="L28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M28">
+        <v>0.98040000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>2700</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29">
+        <v>1.442167</v>
+      </c>
+      <c r="E29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29">
+        <v>0.98070000000000002</v>
+      </c>
+      <c r="H29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>2700</v>
+      </c>
+      <c r="J29" t="s">
+        <v>103</v>
+      </c>
+      <c r="K29">
+        <v>3.6358855000000001</v>
+      </c>
+      <c r="L29" t="s">
+        <v>104</v>
+      </c>
+      <c r="M29">
+        <v>0.98209999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>2800</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30">
+        <v>1.6591473999999999</v>
+      </c>
+      <c r="E30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="H30" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>2800</v>
+      </c>
+      <c r="J30" t="s">
+        <v>103</v>
+      </c>
+      <c r="K30">
+        <v>1.8152013</v>
+      </c>
+      <c r="L30" t="s">
+        <v>104</v>
+      </c>
+      <c r="M30">
+        <v>0.98250000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>2900</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31">
+        <v>5.5154310000000004</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31">
+        <v>0.98080000000000001</v>
+      </c>
+      <c r="H31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>2900</v>
+      </c>
+      <c r="J31" t="s">
+        <v>103</v>
+      </c>
+      <c r="K31">
+        <v>1.3718376000000001</v>
+      </c>
+      <c r="L31" t="s">
+        <v>104</v>
+      </c>
+      <c r="M31">
+        <v>0.98270000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="H32" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix 'sd' and 'mom' (mu, mom) init value
</commit_message>
<xml_diff>
--- a/compare-mnist.xlsx
+++ b/compare-mnist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
+    <workbookView xWindow="2960" yWindow="0" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,105 +226,6 @@
     <t>2m39.523s</t>
   </si>
   <si>
-    <t>472.33603 acc=</t>
-  </si>
-  <si>
-    <t>87.73349 acc=</t>
-  </si>
-  <si>
-    <t>54.761047 acc=</t>
-  </si>
-  <si>
-    <t>45.483 acc=</t>
-  </si>
-  <si>
-    <t>28.407032 acc=</t>
-  </si>
-  <si>
-    <t>18.546188 acc=</t>
-  </si>
-  <si>
-    <t>20.092958 acc=</t>
-  </si>
-  <si>
-    <t>17.823841 acc=</t>
-  </si>
-  <si>
-    <t>20.437433 acc=</t>
-  </si>
-  <si>
-    <t>7.4117303 acc=</t>
-  </si>
-  <si>
-    <t>14.445073 acc=</t>
-  </si>
-  <si>
-    <t>10.841881 acc=</t>
-  </si>
-  <si>
-    <t>16.820187 acc=</t>
-  </si>
-  <si>
-    <t>8.839632 acc=</t>
-  </si>
-  <si>
-    <t>7.6102543 acc=</t>
-  </si>
-  <si>
-    <t>9.938401 acc=</t>
-  </si>
-  <si>
-    <t>5.6252804 acc=</t>
-  </si>
-  <si>
-    <t>2.3085408 acc=</t>
-  </si>
-  <si>
-    <t>1.1648536 acc=</t>
-  </si>
-  <si>
-    <t>8.679963 acc=</t>
-  </si>
-  <si>
-    <t>7.2759576 acc=</t>
-  </si>
-  <si>
-    <t>5.4800506 acc=</t>
-  </si>
-  <si>
-    <t>6.191964 acc=</t>
-  </si>
-  <si>
-    <t>0.9176717 acc=</t>
-  </si>
-  <si>
-    <t>6.5200233 acc=</t>
-  </si>
-  <si>
-    <t>2.6826854 acc=</t>
-  </si>
-  <si>
-    <t>5.359622 acc=</t>
-  </si>
-  <si>
-    <t>3.6358855 acc=</t>
-  </si>
-  <si>
-    <t>1.8152013 acc=</t>
-  </si>
-  <si>
-    <t>1.3718376 acc=</t>
-  </si>
-  <si>
-    <t>5m36.304s</t>
-  </si>
-  <si>
-    <t>15m48.703s</t>
-  </si>
-  <si>
-    <t>2m40.909s</t>
-  </si>
-  <si>
     <t>Adam</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -353,6 +254,105 @@
   <si>
     <t>SDProp Acc</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>607.50793 acc=</t>
+  </si>
+  <si>
+    <t>25.119167 acc=</t>
+  </si>
+  <si>
+    <t>25.625402 acc=</t>
+  </si>
+  <si>
+    <t>19.004848 acc=</t>
+  </si>
+  <si>
+    <t>25.825266 acc=</t>
+  </si>
+  <si>
+    <t>15.177422 acc=</t>
+  </si>
+  <si>
+    <t>13.506539 acc=</t>
+  </si>
+  <si>
+    <t>8.753591 acc=</t>
+  </si>
+  <si>
+    <t>8.180258 acc=</t>
+  </si>
+  <si>
+    <t>4.885234 acc=</t>
+  </si>
+  <si>
+    <t>9.408338 acc=</t>
+  </si>
+  <si>
+    <t>8.384188 acc=</t>
+  </si>
+  <si>
+    <t>13.498153 acc=</t>
+  </si>
+  <si>
+    <t>5.162536 acc=</t>
+  </si>
+  <si>
+    <t>4.1423407 acc=</t>
+  </si>
+  <si>
+    <t>6.944345 acc=</t>
+  </si>
+  <si>
+    <t>2.6742256 acc=</t>
+  </si>
+  <si>
+    <t>1.323509 acc=</t>
+  </si>
+  <si>
+    <t>1.9286346 acc=</t>
+  </si>
+  <si>
+    <t>3.0258079 acc=</t>
+  </si>
+  <si>
+    <t>2.185761 acc=</t>
+  </si>
+  <si>
+    <t>2.2570162 acc=</t>
+  </si>
+  <si>
+    <t>2.565874 acc=</t>
+  </si>
+  <si>
+    <t>3.8926957 acc=</t>
+  </si>
+  <si>
+    <t>3.4811668 acc=</t>
+  </si>
+  <si>
+    <t>8.755626 acc=</t>
+  </si>
+  <si>
+    <t>2.6696956 acc=</t>
+  </si>
+  <si>
+    <t>8.219879 acc=</t>
+  </si>
+  <si>
+    <t>3.756762 acc=</t>
+  </si>
+  <si>
+    <t>2.5063317 acc=</t>
+  </si>
+  <si>
+    <t>5m35.011s</t>
+  </si>
+  <si>
+    <t>15m51.091s</t>
+  </si>
+  <si>
+    <t>2m34.909s</t>
   </si>
 </sst>
 </file>
@@ -607,94 +607,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.1328</c:v>
+                  <c:v>0.101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7208</c:v>
+                  <c:v>0.8977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8393</c:v>
+                  <c:v>0.9221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8816</c:v>
+                  <c:v>0.9372</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9156</c:v>
+                  <c:v>0.9422</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9221</c:v>
+                  <c:v>0.952</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.932</c:v>
+                  <c:v>0.9564</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9417</c:v>
+                  <c:v>0.9603</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9485</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.9564</c:v>
+                  <c:v>0.9657</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.9621</c:v>
+                  <c:v>0.9698</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.964</c:v>
+                  <c:v>0.9715</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.9683</c:v>
+                  <c:v>0.9727</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.9704</c:v>
+                  <c:v>0.9702</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9668</c:v>
+                  <c:v>0.9743</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.9736</c:v>
+                  <c:v>0.9745</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.9748</c:v>
+                  <c:v>0.9783</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9765</c:v>
+                  <c:v>0.9782</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.9763</c:v>
+                  <c:v>0.9802</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.9787</c:v>
+                  <c:v>0.9783</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.9785</c:v>
+                  <c:v>0.9798</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.9793</c:v>
+                  <c:v>0.9794</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9796</c:v>
+                  <c:v>0.9823</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9817</c:v>
+                  <c:v>0.9809</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.9813</c:v>
+                  <c:v>0.9819</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.982</c:v>
+                  <c:v>0.9808</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.9804</c:v>
+                  <c:v>0.9846</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.9821</c:v>
+                  <c:v>0.9838</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.9825</c:v>
+                  <c:v>0.9841</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.9827</c:v>
+                  <c:v>0.9824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -711,11 +711,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2140572184"/>
-        <c:axId val="2140609176"/>
+        <c:axId val="2091386904"/>
+        <c:axId val="2091384280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2140572184"/>
+        <c:axId val="2091386904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,7 +724,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140609176"/>
+        <c:crossAx val="2091384280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -732,10 +732,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140609176"/>
+        <c:axId val="2091384280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
+          <c:min val="0.8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -744,7 +745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140572184"/>
+        <c:crossAx val="2091386904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -928,94 +929,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>472.33603</c:v>
+                  <c:v>607.50793</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.73349</c:v>
+                  <c:v>25.119167</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.761047</c:v>
+                  <c:v>25.625402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.483</c:v>
+                  <c:v>19.004848</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.407032</c:v>
+                  <c:v>25.825266</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.546188</c:v>
+                  <c:v>15.177422</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.092958</c:v>
+                  <c:v>13.506539</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.823841</c:v>
+                  <c:v>8.753591</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.437433</c:v>
+                  <c:v>8.180258</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.4117303</c:v>
+                  <c:v>4.885234</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.445073</c:v>
+                  <c:v>9.408338000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.841881</c:v>
+                  <c:v>8.384188</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.820187</c:v>
+                  <c:v>13.498153</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.839632</c:v>
+                  <c:v>5.162536</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.6102543</c:v>
+                  <c:v>4.1423407</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.938401000000001</c:v>
+                  <c:v>6.944345</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.6252804</c:v>
+                  <c:v>2.6742256</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3085408</c:v>
+                  <c:v>1.323509</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1648536</c:v>
+                  <c:v>1.9286346</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.679963000000001</c:v>
+                  <c:v>3.0258079</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.2759576</c:v>
+                  <c:v>2.185761</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.4800506</c:v>
+                  <c:v>2.2570162</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.191964</c:v>
+                  <c:v>2.565874</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9176717</c:v>
+                  <c:v>3.8926957</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.5200233</c:v>
+                  <c:v>3.4811668</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.6826854</c:v>
+                  <c:v>8.755626</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.359622</c:v>
+                  <c:v>2.6696956</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.6358855</c:v>
+                  <c:v>8.219879000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.8152013</c:v>
+                  <c:v>3.756762</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.3718376</c:v>
+                  <c:v>2.5063317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1032,11 +1033,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2146118024"/>
-        <c:axId val="2146121112"/>
+        <c:axId val="2091464456"/>
+        <c:axId val="2091467432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2146118024"/>
+        <c:axId val="2091464456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146121112"/>
+        <c:crossAx val="2091467432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1053,7 +1054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146121112"/>
+        <c:axId val="2091467432"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1065,7 +1066,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146118024"/>
+        <c:crossAx val="2091464456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1482,17 +1483,17 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:G36"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="D1" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1515,10 +1516,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="I2">
-        <v>0.1328</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1541,10 +1542,10 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I3">
-        <v>0.7208</v>
+        <v>0.89770000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1567,10 +1568,10 @@
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="I4">
-        <v>0.83930000000000005</v>
+        <v>0.92210000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1593,10 +1594,10 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="I5">
-        <v>0.88160000000000005</v>
+        <v>0.93720000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1619,10 +1620,10 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="I6">
-        <v>0.91559999999999997</v>
+        <v>0.94220000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1645,10 +1646,10 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I7">
-        <v>0.92210000000000003</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1671,10 +1672,10 @@
         <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I8">
-        <v>0.93200000000000005</v>
+        <v>0.95640000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1697,10 +1698,10 @@
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I9">
-        <v>0.94169999999999998</v>
+        <v>0.96030000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1723,10 +1724,10 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="I10">
-        <v>0.94850000000000001</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1749,10 +1750,10 @@
         <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I11">
-        <v>0.95640000000000003</v>
+        <v>0.9657</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1775,10 +1776,10 @@
         <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I12">
-        <v>0.96209999999999996</v>
+        <v>0.9698</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1801,10 +1802,10 @@
         <v>23</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I13">
-        <v>0.96399999999999997</v>
+        <v>0.97150000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1827,10 +1828,10 @@
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I14">
-        <v>0.96830000000000005</v>
+        <v>0.97270000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1853,10 +1854,10 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="I15">
-        <v>0.97040000000000004</v>
+        <v>0.97019999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1879,10 +1880,10 @@
         <v>29</v>
       </c>
       <c r="H16" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I16">
-        <v>0.96679999999999999</v>
+        <v>0.97430000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1905,10 +1906,10 @@
         <v>31</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="I17">
-        <v>0.97360000000000002</v>
+        <v>0.97450000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1931,10 +1932,10 @@
         <v>33</v>
       </c>
       <c r="H18" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="I18">
-        <v>0.9748</v>
+        <v>0.97829999999999995</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1957,10 +1958,10 @@
         <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="I19">
-        <v>0.97650000000000003</v>
+        <v>0.97819999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1983,10 +1984,10 @@
         <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I20">
-        <v>0.97629999999999995</v>
+        <v>0.98019999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2009,10 +2010,10 @@
         <v>39</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="I21">
-        <v>0.97870000000000001</v>
+        <v>0.97829999999999995</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2035,10 +2036,10 @@
         <v>41</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="I22">
-        <v>0.97850000000000004</v>
+        <v>0.9798</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2061,10 +2062,10 @@
         <v>43</v>
       </c>
       <c r="H23" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="I23">
-        <v>0.97929999999999995</v>
+        <v>0.97940000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2087,10 +2088,10 @@
         <v>45</v>
       </c>
       <c r="H24" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I24">
-        <v>0.97960000000000003</v>
+        <v>0.98229999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2113,10 +2114,10 @@
         <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="I25">
-        <v>0.98170000000000002</v>
+        <v>0.98089999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2139,10 +2140,10 @@
         <v>49</v>
       </c>
       <c r="H26" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I26">
-        <v>0.98129999999999995</v>
+        <v>0.9819</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2165,10 +2166,10 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I27">
-        <v>0.98199999999999998</v>
+        <v>0.98080000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2191,10 +2192,10 @@
         <v>53</v>
       </c>
       <c r="H28" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I28">
-        <v>0.98040000000000005</v>
+        <v>0.98460000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2217,10 +2218,10 @@
         <v>55</v>
       </c>
       <c r="H29" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="I29">
-        <v>0.98209999999999997</v>
+        <v>0.98380000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2243,10 +2244,10 @@
         <v>57</v>
       </c>
       <c r="H30" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="I30">
-        <v>0.98250000000000004</v>
+        <v>0.98409999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2269,10 +2270,10 @@
         <v>59</v>
       </c>
       <c r="H31" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I31">
-        <v>0.98270000000000002</v>
+        <v>0.98240000000000005</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2286,7 +2287,7 @@
         <v>61</v>
       </c>
       <c r="G32">
-        <v>0.98399999999999999</v>
+        <v>0.98509999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2300,7 +2301,7 @@
         <v>62</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2314,7 +2315,7 @@
         <v>64</v>
       </c>
       <c r="G35" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2328,7 +2329,7 @@
         <v>66</v>
       </c>
       <c r="G36" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2350,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="K1" activeCellId="1" sqref="D1:D31 K1:K31"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2371,16 +2372,16 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="D1" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="K1" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="M1" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -2391,13 +2392,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>565.45734000000004</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F2">
         <v>5.4600000000000003E-2</v>
@@ -2409,16 +2410,16 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K2">
-        <v>472.33602999999999</v>
+        <v>607.50792999999999</v>
       </c>
       <c r="L2" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M2">
-        <v>0.1328</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2429,13 +2430,13 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D3">
         <v>68.185615999999996</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>0.84709999999999996</v>
@@ -2447,16 +2448,16 @@
         <v>100</v>
       </c>
       <c r="J3" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K3">
-        <v>87.733490000000003</v>
+        <v>25.119167000000001</v>
       </c>
       <c r="L3" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M3">
-        <v>0.7208</v>
+        <v>0.89770000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2467,13 +2468,13 @@
         <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <v>39.780589999999997</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F4">
         <v>0.9103</v>
@@ -2485,16 +2486,16 @@
         <v>200</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K4">
-        <v>54.761046999999998</v>
+        <v>25.625402000000001</v>
       </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M4">
-        <v>0.83930000000000005</v>
+        <v>0.92210000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2505,13 +2506,13 @@
         <v>300</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>30.144241000000001</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F5">
         <v>0.92879999999999996</v>
@@ -2523,16 +2524,16 @@
         <v>300</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K5">
-        <v>45.482999999999997</v>
+        <v>19.004847999999999</v>
       </c>
       <c r="L5" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M5">
-        <v>0.88160000000000005</v>
+        <v>0.93720000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2543,13 +2544,13 @@
         <v>400</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>27.758614000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F6">
         <v>0.93840000000000001</v>
@@ -2561,16 +2562,16 @@
         <v>400</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K6">
-        <v>28.407032000000001</v>
+        <v>25.825265999999999</v>
       </c>
       <c r="L6" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M6">
-        <v>0.91559999999999997</v>
+        <v>0.94220000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2581,13 +2582,13 @@
         <v>500</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>12.258660000000001</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F7">
         <v>0.94710000000000005</v>
@@ -2599,16 +2600,16 @@
         <v>500</v>
       </c>
       <c r="J7" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K7">
-        <v>18.546188000000001</v>
+        <v>15.177422</v>
       </c>
       <c r="L7" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M7">
-        <v>0.92210000000000003</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2619,13 +2620,13 @@
         <v>600</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>12.17146</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F8">
         <v>0.95020000000000004</v>
@@ -2637,16 +2638,16 @@
         <v>600</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K8">
-        <v>20.092957999999999</v>
+        <v>13.506539</v>
       </c>
       <c r="L8" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M8">
-        <v>0.93200000000000005</v>
+        <v>0.95640000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2657,13 +2658,13 @@
         <v>700</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D9">
         <v>13.063127</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F9">
         <v>0.95589999999999997</v>
@@ -2675,16 +2676,16 @@
         <v>700</v>
       </c>
       <c r="J9" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K9">
-        <v>17.823841000000002</v>
+        <v>8.7535910000000001</v>
       </c>
       <c r="L9" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M9">
-        <v>0.94169999999999998</v>
+        <v>0.96030000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2695,13 +2696,13 @@
         <v>800</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D10">
         <v>13.2274475</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F10">
         <v>0.96050000000000002</v>
@@ -2713,16 +2714,16 @@
         <v>800</v>
       </c>
       <c r="J10" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K10">
-        <v>20.437432999999999</v>
+        <v>8.1802580000000003</v>
       </c>
       <c r="L10" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M10">
-        <v>0.94850000000000001</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2733,13 +2734,13 @@
         <v>900</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <v>9.6371990000000007</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F11">
         <v>0.96279999999999999</v>
@@ -2751,16 +2752,16 @@
         <v>900</v>
       </c>
       <c r="J11" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K11">
-        <v>7.4117303000000003</v>
+        <v>4.8852339999999996</v>
       </c>
       <c r="L11" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M11">
-        <v>0.95640000000000003</v>
+        <v>0.9657</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2771,13 +2772,13 @@
         <v>1000</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D12">
         <v>6.3767719999999999</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F12">
         <v>0.96689999999999998</v>
@@ -2789,16 +2790,16 @@
         <v>1000</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K12">
-        <v>14.445073000000001</v>
+        <v>9.4083380000000005</v>
       </c>
       <c r="L12" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M12">
-        <v>0.96209999999999996</v>
+        <v>0.9698</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2809,13 +2810,13 @@
         <v>1100</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D13">
         <v>13.041093</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F13">
         <v>0.96750000000000003</v>
@@ -2827,16 +2828,16 @@
         <v>1100</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K13">
-        <v>10.841881000000001</v>
+        <v>8.384188</v>
       </c>
       <c r="L13" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M13">
-        <v>0.96399999999999997</v>
+        <v>0.97150000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -2847,13 +2848,13 @@
         <v>1200</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D14">
         <v>20.754767999999999</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F14">
         <v>0.97009999999999996</v>
@@ -2865,16 +2866,16 @@
         <v>1200</v>
       </c>
       <c r="J14" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K14">
-        <v>16.820187000000001</v>
+        <v>13.498153</v>
       </c>
       <c r="L14" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M14">
-        <v>0.96830000000000005</v>
+        <v>0.97270000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -2885,13 +2886,13 @@
         <v>1300</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D15">
         <v>9.1106200000000008</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F15">
         <v>0.96930000000000005</v>
@@ -2903,16 +2904,16 @@
         <v>1300</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K15">
-        <v>8.8396319999999999</v>
+        <v>5.1625360000000002</v>
       </c>
       <c r="L15" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M15">
-        <v>0.97040000000000004</v>
+        <v>0.97019999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -2923,13 +2924,13 @@
         <v>1400</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D16">
         <v>7.3511033000000001</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F16">
         <v>0.97219999999999995</v>
@@ -2941,16 +2942,16 @@
         <v>1400</v>
       </c>
       <c r="J16" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K16">
-        <v>7.6102543000000002</v>
+        <v>4.1423407000000001</v>
       </c>
       <c r="L16" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M16">
-        <v>0.96679999999999999</v>
+        <v>0.97430000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2961,13 +2962,13 @@
         <v>1500</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D17">
         <v>2.2841954000000002</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F17">
         <v>0.97040000000000004</v>
@@ -2979,16 +2980,16 @@
         <v>1500</v>
       </c>
       <c r="J17" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K17">
-        <v>9.9384010000000007</v>
+        <v>6.9443450000000002</v>
       </c>
       <c r="L17" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M17">
-        <v>0.97360000000000002</v>
+        <v>0.97450000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -2999,13 +3000,13 @@
         <v>1600</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D18">
         <v>10.884306</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F18">
         <v>0.97389999999999999</v>
@@ -3017,16 +3018,16 @@
         <v>1600</v>
       </c>
       <c r="J18" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K18">
-        <v>5.6252804000000003</v>
+        <v>2.6742256000000002</v>
       </c>
       <c r="L18" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M18">
-        <v>0.9748</v>
+        <v>0.97829999999999995</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -3037,13 +3038,13 @@
         <v>1700</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D19">
         <v>17.515066000000001</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F19">
         <v>0.97509999999999997</v>
@@ -3055,16 +3056,16 @@
         <v>1700</v>
       </c>
       <c r="J19" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K19">
-        <v>2.3085407999999998</v>
+        <v>1.323509</v>
       </c>
       <c r="L19" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M19">
-        <v>0.97650000000000003</v>
+        <v>0.97819999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -3075,13 +3076,13 @@
         <v>1800</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>9.4372469999999993</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F20">
         <v>0.97550000000000003</v>
@@ -3093,16 +3094,16 @@
         <v>1800</v>
       </c>
       <c r="J20" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K20">
-        <v>1.1648536</v>
+        <v>1.9286346000000001</v>
       </c>
       <c r="L20" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M20">
-        <v>0.97629999999999995</v>
+        <v>0.98019999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -3113,13 +3114,13 @@
         <v>1900</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D21">
         <v>8.6005020000000005</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F21">
         <v>0.97509999999999997</v>
@@ -3131,16 +3132,16 @@
         <v>1900</v>
       </c>
       <c r="J21" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K21">
-        <v>8.6799630000000008</v>
+        <v>3.0258079000000002</v>
       </c>
       <c r="L21" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M21">
-        <v>0.97870000000000001</v>
+        <v>0.97829999999999995</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -3151,13 +3152,13 @@
         <v>2000</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D22">
         <v>3.1273580000000001</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F22">
         <v>0.97789999999999999</v>
@@ -3169,16 +3170,16 @@
         <v>2000</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K22">
-        <v>7.2759575999999999</v>
+        <v>2.1857609999999998</v>
       </c>
       <c r="L22" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M22">
-        <v>0.97850000000000004</v>
+        <v>0.9798</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -3189,13 +3190,13 @@
         <v>2100</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D23">
         <v>4.3089924000000002</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F23">
         <v>0.97699999999999998</v>
@@ -3207,16 +3208,16 @@
         <v>2100</v>
       </c>
       <c r="J23" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K23">
-        <v>5.4800506000000002</v>
+        <v>2.2570161999999998</v>
       </c>
       <c r="L23" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M23">
-        <v>0.97929999999999995</v>
+        <v>0.97940000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -3227,13 +3228,13 @@
         <v>2200</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D24">
         <v>2.5774632</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F24">
         <v>0.97760000000000002</v>
@@ -3245,16 +3246,16 @@
         <v>2200</v>
       </c>
       <c r="J24" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K24">
-        <v>6.1919639999999996</v>
+        <v>2.565874</v>
       </c>
       <c r="L24" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M24">
-        <v>0.97960000000000003</v>
+        <v>0.98229999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -3265,13 +3266,13 @@
         <v>2300</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D25">
         <v>12.162725</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F25">
         <v>0.9788</v>
@@ -3283,16 +3284,16 @@
         <v>2300</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K25">
-        <v>0.91767169999999998</v>
+        <v>3.8926957</v>
       </c>
       <c r="L25" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M25">
-        <v>0.98170000000000002</v>
+        <v>0.98089999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -3303,13 +3304,13 @@
         <v>2400</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D26">
         <v>3.4844575</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F26">
         <v>0.97919999999999996</v>
@@ -3321,16 +3322,16 @@
         <v>2400</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K26">
-        <v>6.5200233000000001</v>
+        <v>3.4811668</v>
       </c>
       <c r="L26" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M26">
-        <v>0.98129999999999995</v>
+        <v>0.9819</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -3341,13 +3342,13 @@
         <v>2500</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D27">
         <v>6.1178435999999996</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F27">
         <v>0.97799999999999998</v>
@@ -3359,16 +3360,16 @@
         <v>2500</v>
       </c>
       <c r="J27" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K27">
-        <v>2.6826854</v>
+        <v>8.7556259999999995</v>
       </c>
       <c r="L27" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M27">
-        <v>0.98199999999999998</v>
+        <v>0.98080000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3379,13 +3380,13 @@
         <v>2600</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D28">
         <v>6.9269610000000004</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F28">
         <v>0.98060000000000003</v>
@@ -3397,16 +3398,16 @@
         <v>2600</v>
       </c>
       <c r="J28" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K28">
-        <v>5.3596219999999999</v>
+        <v>2.6696955999999998</v>
       </c>
       <c r="L28" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M28">
-        <v>0.98040000000000005</v>
+        <v>0.98460000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -3417,13 +3418,13 @@
         <v>2700</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>1.442167</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F29">
         <v>0.98070000000000002</v>
@@ -3435,16 +3436,16 @@
         <v>2700</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K29">
-        <v>3.6358855000000001</v>
+        <v>8.2198790000000006</v>
       </c>
       <c r="L29" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M29">
-        <v>0.98209999999999997</v>
+        <v>0.98380000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -3455,13 +3456,13 @@
         <v>2800</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D30">
         <v>1.6591473999999999</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F30">
         <v>0.98109999999999997</v>
@@ -3473,16 +3474,16 @@
         <v>2800</v>
       </c>
       <c r="J30" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K30">
-        <v>1.8152013</v>
+        <v>3.7567620000000002</v>
       </c>
       <c r="L30" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M30">
-        <v>0.98250000000000004</v>
+        <v>0.98409999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -3493,13 +3494,13 @@
         <v>2900</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D31">
         <v>5.5154310000000004</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F31">
         <v>0.98080000000000001</v>
@@ -3511,16 +3512,16 @@
         <v>2900</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="K31">
-        <v>1.3718376000000001</v>
+        <v>2.5063317000000001</v>
       </c>
       <c r="L31" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="M31">
-        <v>0.98270000000000002</v>
+        <v>0.98240000000000005</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -3534,7 +3535,7 @@
         <v>61</v>
       </c>
       <c r="I32">
-        <v>0.98399999999999999</v>
+        <v>0.98509999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3548,7 +3549,7 @@
         <v>62</v>
       </c>
       <c r="I34" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3562,7 +3563,7 @@
         <v>64</v>
       </c>
       <c r="I35" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3576,7 +3577,7 @@
         <v>66</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>